<commit_message>
Add Icrack and Mcrack to section inputs
* Sections now takes two more input for cracked beam.
</commit_message>
<xml_diff>
--- a/Input/Inputs.xlsx
+++ b/Input/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\analysis-engine-3d\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A999EE3B-FF3C-4E82-A046-73F8C16F87CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACACEE8-5451-4756-9BCB-D963449A466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
+    <workbookView xWindow="30360" yWindow="2460" windowWidth="16200" windowHeight="9345" activeTab="1" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Node ID</t>
   </si>
@@ -126,12 +126,6 @@
     <t>Area, A (m^2)</t>
   </si>
   <si>
-    <t xml:space="preserve">Moment of Inertian in Local Y, Iy (m^4) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moment of Inertian in Local Z, Iz (m^4) </t>
-  </si>
-  <si>
     <t>Fx</t>
   </si>
   <si>
@@ -145,6 +139,18 @@
   </si>
   <si>
     <t xml:space="preserve">Node ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moment of Inertia in Local Z, Iz (m^4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moment of Inertia in Local Y, Iy (m^4) </t>
+  </si>
+  <si>
+    <t>Cracked Moment of Inertia (m^4)</t>
+  </si>
+  <si>
+    <t>Cracking Moment (kN-m)</t>
   </si>
 </sst>
 </file>
@@ -600,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1968B7-5424-4C36-8505-5F3C4CDAA493}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -697,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31138835-7400-4358-88E1-2D9D6D88288C}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -862,10 +868,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDD292-B116-45BF-A498-8DFDE4EC10A0}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,9 +880,11 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -887,10 +895,16 @@
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -913,19 +927,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
example input with an experiment result
</commit_message>
<xml_diff>
--- a/Input/Inputs.xlsx
+++ b/Input/Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\analysis-engine-3d\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACACEE8-5451-4756-9BCB-D963449A466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0175F78-1FCC-4A4C-8EB3-2B0955F02D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="2460" windowWidth="16200" windowHeight="9345" activeTab="1" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="12735" firstSheet="3" activeTab="6" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Node ID</t>
   </si>
@@ -126,6 +126,12 @@
     <t>Area, A (m^2)</t>
   </si>
   <si>
+    <t xml:space="preserve">Moment of Inertian in Local Y, Iy (m^4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moment of Inertian in Local Z, Iz (m^4) </t>
+  </si>
+  <si>
     <t>Fx</t>
   </si>
   <si>
@@ -138,19 +144,19 @@
     <t>Load ID</t>
   </si>
   <si>
+    <t>Mesh Count in X direction</t>
+  </si>
+  <si>
+    <t>Mesh Count in Y direction</t>
+  </si>
+  <si>
     <t xml:space="preserve">Node ID </t>
   </si>
   <si>
-    <t xml:space="preserve">Moment of Inertia in Local Z, Iz (m^4) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moment of Inertia in Local Y, Iy (m^4) </t>
-  </si>
-  <si>
-    <t>Cracked Moment of Inertia (m^4)</t>
-  </si>
-  <si>
-    <t>Cracking Moment (kN-m)</t>
+    <t>Icr</t>
+  </si>
+  <si>
+    <t>Mcr</t>
   </si>
 </sst>
 </file>
@@ -219,7 +225,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CB60D2-9CEA-4AF6-BBFE-14189615886A}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -574,13 +580,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,12 +594,222 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.65</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.8</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.95</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1.25</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1.4</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1.55</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1.7</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1.85</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2.15</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2.4</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2.5</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
         <v>0</v>
       </c>
     </row>
@@ -604,10 +820,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1968B7-5424-4C36-8505-5F3C4CDAA493}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -673,13 +889,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -691,7 +907,449 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -701,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31138835-7400-4358-88E1-2D9D6D88288C}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,34 +1404,14 @@
       <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>0.6</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -783,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06747EAA-2B3E-4129-BECE-62A3CA8D8DBC}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,6 +1457,366 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>19</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -829,7 +1827,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,10 +1853,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200000</v>
+        <v>29048889.823881391</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -868,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDD292-B116-45BF-A498-8DFDE4EC10A0}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,8 +1878,7 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -895,29 +1892,53 @@
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.04</v>
+      </c>
+      <c r="C2">
+        <v>1.3333333333333337E-4</v>
+      </c>
+      <c r="D2">
+        <v>1.3333333333333337E-4</v>
+      </c>
+      <c r="E2">
+        <v>1.3333333333333337E-4</v>
+      </c>
+      <c r="F2">
+        <v>4.7688173852848175E-5</v>
+      </c>
+      <c r="G2">
+        <v>5.1093082810798487</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AED2E2A-F152-4D08-9EBD-35E68852C800}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,19 +1948,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
@@ -951,7 +1972,216 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-8.1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>-8.1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-8.1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-8.1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>-8.1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-8.1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>-8.1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>-8.1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the input method and xls file
</commit_message>
<xml_diff>
--- a/Input/Inputs.xlsx
+++ b/Input/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\analysis-engine-3d\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A999EE3B-FF3C-4E82-A046-73F8C16F87CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BA8BBB-F17C-4EEE-8F07-173C8285206F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Materials" sheetId="5" r:id="rId5"/>
     <sheet name="Sections" sheetId="6" r:id="rId6"/>
     <sheet name="Nodal Load" sheetId="7" r:id="rId7"/>
+    <sheet name="Arc Length Parameters" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Node ID</t>
   </si>
@@ -144,7 +145,31 @@
     <t>Load ID</t>
   </si>
   <si>
+    <t>Mesh Count in X direction</t>
+  </si>
+  <si>
+    <t>Mesh Count in Y direction</t>
+  </si>
+  <si>
     <t xml:space="preserve">Node ID </t>
+  </si>
+  <si>
+    <t>Phi</t>
+  </si>
+  <si>
+    <t>Tolerance</t>
+  </si>
+  <si>
+    <t>Maximum Iteration Number</t>
+  </si>
+  <si>
+    <t>Number of Increment</t>
+  </si>
+  <si>
+    <t>Arc Length</t>
+  </si>
+  <si>
+    <t>Strain Type</t>
   </si>
 </sst>
 </file>
@@ -190,11 +215,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CB60D2-9CEA-4AF6-BBFE-14189615886A}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +584,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -568,13 +598,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -582,12 +612,40 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
     </row>
@@ -598,10 +656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1968B7-5424-4C36-8505-5F3C4CDAA493}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,24 +725,128 @@
         <v>2</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
     </row>
@@ -695,10 +857,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31138835-7400-4358-88E1-2D9D6D88288C}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,34 +902,14 @@
       <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>0.6</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -777,10 +919,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06747EAA-2B3E-4129-BECE-62A3CA8D8DBC}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,6 +955,106 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -823,7 +1065,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,10 +1091,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200000</v>
+        <v>500000</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -862,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDD292-B116-45BF-A498-8DFDE4EC10A0}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,6 +1135,23 @@
         <v>29</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -900,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AED2E2A-F152-4D08-9EBD-35E68852C800}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +1175,7 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -935,6 +1194,96 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F2443A-431B-4692-8FE1-7CACE58C740C}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>10^(-7)</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add moment curvature curve to input file and input reader
</commit_message>
<xml_diff>
--- a/Input/Inputs.xlsx
+++ b/Input/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\analysis-engine-3d\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0175F78-1FCC-4A4C-8EB3-2B0955F02D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267D904C-E42F-497D-91EB-C0937270964A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="12735" firstSheet="3" activeTab="6" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Materials" sheetId="5" r:id="rId5"/>
     <sheet name="Sections" sheetId="6" r:id="rId6"/>
     <sheet name="Nodal Load" sheetId="7" r:id="rId7"/>
+    <sheet name="curve1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Node ID</t>
   </si>
@@ -157,6 +158,18 @@
   </si>
   <si>
     <t>Mcr</t>
+  </si>
+  <si>
+    <t>curve1</t>
+  </si>
+  <si>
+    <t>Curvature</t>
+  </si>
+  <si>
+    <t>Moment</t>
+  </si>
+  <si>
+    <t>Moment Curvature Curve Sheet Name</t>
   </si>
 </sst>
 </file>
@@ -521,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CB60D2-9CEA-4AF6-BBFE-14189615886A}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -608,7 +621,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -622,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -636,7 +649,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -650,7 +663,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.95</v>
+        <v>0.7</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -664,7 +677,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1.1000000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -678,7 +691,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1.25</v>
+        <v>0.9</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -692,7 +705,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -706,7 +719,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1.55</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -720,7 +733,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1.7</v>
+        <v>1.2</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -734,7 +747,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1.85</v>
+        <v>1.3</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -748,7 +761,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -762,7 +775,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>2.15</v>
+        <v>1.5</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -776,7 +789,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2.2999999999999998</v>
+        <v>1.6</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -790,7 +803,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>2.4</v>
+        <v>1.7</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -804,12 +817,40 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1.9</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>0</v>
       </c>
     </row>
@@ -820,10 +861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1968B7-5424-4C36-8505-5F3C4CDAA493}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1337,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1349,6 +1390,58 @@
         <v>1</v>
       </c>
       <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>0</v>
       </c>
     </row>
@@ -1421,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06747EAA-2B3E-4129-BECE-62A3CA8D8DBC}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,6 +1907,46 @@
         <v>1</v>
       </c>
       <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>1</v>
       </c>
     </row>
@@ -1866,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDD292-B116-45BF-A498-8DFDE4EC10A0}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,9 +2012,10 @@
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1903,8 +2037,11 @@
       <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1925,6 +2062,9 @@
       </c>
       <c r="G2">
         <v>5.1093082810798487</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1935,10 +2075,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AED2E2A-F152-4D08-9EBD-35E68852C800}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1977,13 +2117,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>-8.1</v>
+        <v>-20</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2003,13 +2143,14 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>-8.1</v>
+        <f>D2</f>
+        <v>-20</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2029,13 +2170,14 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>-8.1</v>
+        <f t="shared" ref="D4:D20" si="0">D3</f>
+        <v>-20</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2055,13 +2197,14 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>-8.1</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2081,13 +2224,14 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>-8.1</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2107,13 +2251,14 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>-8.1</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2133,13 +2278,14 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>-8.1</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2159,24 +2305,322 @@
         <v>8</v>
       </c>
       <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
         <v>17</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>-8.1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>0</v>
       </c>
     </row>
@@ -2184,4 +2628,391 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBB734D-9B9B-45BE-B255-6125F955742A}">
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-0.39660499999999999</v>
+      </c>
+      <c r="B2">
+        <v>-4.17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-0.32197399999999998</v>
+      </c>
+      <c r="B3">
+        <v>-4.78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-0.228134</v>
+      </c>
+      <c r="B4">
+        <v>-5.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-0.20505499999999999</v>
+      </c>
+      <c r="B5">
+        <v>-5.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-0.181115</v>
+      </c>
+      <c r="B6">
+        <v>-5.34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-0.15625500000000001</v>
+      </c>
+      <c r="B7">
+        <v>-5.41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.12990199999999999</v>
+      </c>
+      <c r="B8">
+        <v>-5.41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-0.12650500000000001</v>
+      </c>
+      <c r="B9">
+        <v>-5.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-0.12559000000000001</v>
+      </c>
+      <c r="B10">
+        <v>-5.41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-0.125198</v>
+      </c>
+      <c r="B11">
+        <v>-5.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-0.12474</v>
+      </c>
+      <c r="B12">
+        <v>-5.41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-0.12389</v>
+      </c>
+      <c r="B13">
+        <v>-5.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-0.12304</v>
+      </c>
+      <c r="B14">
+        <v>-5.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-0.116037</v>
+      </c>
+      <c r="B15">
+        <v>-5.38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-0.10882600000000001</v>
+      </c>
+      <c r="B16">
+        <v>-5.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-0.10147399999999999</v>
+      </c>
+      <c r="B17">
+        <v>-5.31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-8.5951E-2</v>
+      </c>
+      <c r="B18">
+        <v>-5.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-6.9375000000000006E-2</v>
+      </c>
+      <c r="B19">
+        <v>-5.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-5.1763000000000003E-2</v>
+      </c>
+      <c r="B20">
+        <v>-4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-3.3103E-2</v>
+      </c>
+      <c r="B21">
+        <v>-4.41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-2.3764E-2</v>
+      </c>
+      <c r="B22">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-1.4063000000000001E-2</v>
+      </c>
+      <c r="B23">
+        <v>-3.96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-6.7889999999999999E-3</v>
+      </c>
+      <c r="B24">
+        <v>-2.21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>6.705E-3</v>
+      </c>
+      <c r="B26">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1.3016E-2</v>
+      </c>
+      <c r="B27">
+        <v>17.34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1.4540000000000001E-2</v>
+      </c>
+      <c r="B28">
+        <v>19.260000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1.6641E-2</v>
+      </c>
+      <c r="B29">
+        <v>20.45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1.7405E-2</v>
+      </c>
+      <c r="B30">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1.8169000000000001E-2</v>
+      </c>
+      <c r="B31">
+        <v>20.54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1.8534999999999999E-2</v>
+      </c>
+      <c r="B32">
+        <v>20.57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1.8932999999999998E-2</v>
+      </c>
+      <c r="B33">
+        <v>20.58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1.9299E-2</v>
+      </c>
+      <c r="B34">
+        <v>20.61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1.9696999999999999E-2</v>
+      </c>
+      <c r="B35">
+        <v>20.59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2.2852000000000001E-2</v>
+      </c>
+      <c r="B36">
+        <v>20.79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3.7246000000000001E-2</v>
+      </c>
+      <c r="B37">
+        <v>21.13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4.4734000000000003E-2</v>
+      </c>
+      <c r="B38">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5.2347999999999999E-2</v>
+      </c>
+      <c r="B39">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5.9759E-2</v>
+      </c>
+      <c r="B40">
+        <v>21.34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6.6999000000000003E-2</v>
+      </c>
+      <c r="B41">
+        <v>21.35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>8.0966999999999997E-2</v>
+      </c>
+      <c r="B42">
+        <v>21.37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>9.4085000000000002E-2</v>
+      </c>
+      <c r="B43">
+        <v>21.33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.140766</v>
+      </c>
+      <c r="B44">
+        <v>21.12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.17944099999999999</v>
+      </c>
+      <c r="B45">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0.25011699999999998</v>
+      </c>
+      <c r="B46">
+        <v>18.87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update getInput method and xls file.
</commit_message>
<xml_diff>
--- a/Input/Inputs.xlsx
+++ b/Input/Inputs.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RazzR\OneDrive\Belgeler\analysis-engine-3d\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\analysis-engine-3d\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86CF452-AD10-4EFF-8F45-8E58279319EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A74BE4-D987-4577-8B1E-F350650908A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="8" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" r:id="rId1"/>
     <sheet name="Supports" sheetId="2" r:id="rId2"/>
     <sheet name="Shell Elements" sheetId="3" r:id="rId3"/>
     <sheet name="Line Elements" sheetId="4" r:id="rId4"/>
-    <sheet name="Materials" sheetId="5" r:id="rId5"/>
-    <sheet name="Sections" sheetId="6" r:id="rId6"/>
-    <sheet name="Nodal Load" sheetId="7" r:id="rId7"/>
-    <sheet name="Arc Length Parameters" sheetId="8" r:id="rId8"/>
+    <sheet name="Nonlinear Line Elements" sheetId="9" r:id="rId5"/>
+    <sheet name="Materials" sheetId="5" r:id="rId6"/>
+    <sheet name="Sections" sheetId="6" r:id="rId7"/>
+    <sheet name="Nodal Load" sheetId="7" r:id="rId8"/>
+    <sheet name="Arc Length Parameters" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Node ID</t>
   </si>
@@ -167,9 +168,6 @@
   </si>
   <si>
     <t>Arc Length</t>
-  </si>
-  <si>
-    <t>Strain Type</t>
   </si>
 </sst>
 </file>
@@ -215,20 +213,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2083,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CB60D2-9CEA-4AF6-BBFE-14189615886A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,12 +2128,26 @@
         <v>2</v>
       </c>
       <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
     </row>
@@ -2144,10 +2158,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1968B7-5424-4C36-8505-5F3C4CDAA493}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,6 +2245,32 @@
         <v>1</v>
       </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
     </row>
@@ -2303,10 +2343,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06747EAA-2B3E-4129-BECE-62A3CA8D8DBC}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,32 +2379,144 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4302C3F1-A01D-4530-9727-3F57C0B6FF8F}">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:T3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03126560-76E5-4179-B42F-5ABF06329966}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2406,7 +2558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDD292-B116-45BF-A498-8DFDE4EC10A0}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2461,12 +2613,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AED2E2A-F152-4D08-9EBD-35E68852C800}">
   <dimension ref="A1:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56:L63"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3469,7 +3621,7 @@
       <c r="N12">
         <v>-230.585417330372</v>
       </c>
-      <c r="U12" s="5"/>
+      <c r="U12" s="4"/>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="K13">
@@ -3483,7 +3635,7 @@
       <c r="K14">
         <v>-5.5</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <v>-4.5058984309434898E-2</v>
       </c>
     </row>
@@ -3491,7 +3643,7 @@
       <c r="K15">
         <v>-11</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="5">
         <v>-9.2767715454101604E-2</v>
       </c>
     </row>
@@ -3821,17 +3973,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F2443A-431B-4692-8FE1-7CACE58C740C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -3855,9 +4007,7 @@
       <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -3867,7 +4017,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="D2">
         <v>1000</v>
@@ -3875,9 +4025,7 @@
       <c r="E2">
         <v>70</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
+      <c r="F2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cantilever with 4-1meter elements (0.1 0 0.00001 1000 55) paramters with order.
</commit_message>
<xml_diff>
--- a/Input/Inputs.xlsx
+++ b/Input/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\analysis-engine-3d\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A74BE4-D987-4577-8B1E-F350650908A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC88934-0DC3-4EB1-8D68-588F8F926018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="8" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" r:id="rId1"/>
@@ -2083,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CB60D2-9CEA-4AF6-BBFE-14189615886A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,26 +2128,12 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
         <v>0</v>
       </c>
     </row>
@@ -2158,10 +2144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1968B7-5424-4C36-8505-5F3C4CDAA493}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,32 +2231,6 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
         <v>0</v>
       </c>
     </row>
@@ -2389,7 +2349,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:T3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2478,24 +2438,6 @@
       <c r="T2" s="7"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -2521,7 +2463,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,7 +2489,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2563,7 +2505,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2596,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2605,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>8.8880000000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2618,7 +2560,7 @@
   <dimension ref="A1:BJ55"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2663,7 +2605,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>-0.01</v>
+        <v>-1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3978,7 +3920,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4017,13 +3959,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D2">
         <v>1000</v>
       </c>
       <c r="E2">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="F2" s="7"/>
     </row>

</xml_diff>

<commit_message>
TwoBeamSnapThroughArcLength 6 meter width 1.2 meter height 2 memeber (0.01 0 0.0001 1000 500) arc length parameters in order.
</commit_message>
<xml_diff>
--- a/Input/Inputs.xlsx
+++ b/Input/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\analysis-engine-3d\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC88934-0DC3-4EB1-8D68-588F8F926018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0ABF2C2-A5F3-44E5-BD94-273337717E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
   </bookViews>
@@ -2083,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CB60D2-9CEA-4AF6-BBFE-14189615886A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,12 +2128,26 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
+        <v>1.2</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
     </row>
@@ -2144,10 +2158,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1968B7-5424-4C36-8505-5F3C4CDAA493}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,7 +2219,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2231,6 +2245,32 @@
         <v>1</v>
       </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
     </row>
@@ -2349,7 +2389,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,6 +2478,24 @@
       <c r="T2" s="7"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -3920,7 +3978,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3953,19 +4011,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="D2">
         <v>1000</v>
       </c>
       <c r="E2">
-        <v>55</v>
+        <v>500</v>
       </c>
       <c r="F2" s="7"/>
     </row>

</xml_diff>

<commit_message>
Take both positive and negative cracking moment
* Cracking moment changes in the section according to bending type. If the moment is positive, use positive cracking moment, if it is negative use the negative cracking moment.

* Input file and input reading logic modified accordingly.
</commit_message>
<xml_diff>
--- a/Input/Inputs.xlsx
+++ b/Input/Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\analysis-engine-3d\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267D904C-E42F-497D-91EB-C0937270964A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DCE46B-DEC4-42EB-AE99-9F022A28A5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{DB72CDF5-9B03-4981-93E0-F1BDE5E8516D}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Node ID</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Icr</t>
   </si>
   <si>
-    <t>Mcr</t>
-  </si>
-  <si>
     <t>curve1</t>
   </si>
   <si>
@@ -170,6 +167,12 @@
   </si>
   <si>
     <t>Moment Curvature Curve Sheet Name</t>
+  </si>
+  <si>
+    <t>Mcr pos</t>
+  </si>
+  <si>
+    <t>Mcr neg</t>
   </si>
 </sst>
 </file>
@@ -1999,10 +2002,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDD292-B116-45BF-A498-8DFDE4EC10A0}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,10 +2015,11 @@
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2035,13 +2039,16 @@
         <v>37</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2063,8 +2070,11 @@
       <c r="G2">
         <v>5.1093082810798487</v>
       </c>
-      <c r="H2" t="s">
-        <v>39</v>
+      <c r="H2">
+        <v>5.1093082810798487</v>
+      </c>
+      <c r="I2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2646,10 +2656,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>